<commit_message>
fix low AL and NC issue for misc plan
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_BART_planInfo_AV2019.xlsx
+++ b/inputs/data_raw/Data_BART_planInfo_AV2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_BART\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0F670D-8AEC-4514-B9FF-2FF74F6757C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6BD958-F4E1-408F-8E4F-BA32771CBE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1500" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init_unrecReturn" sheetId="12" r:id="rId1"/>
@@ -514,12 +514,6 @@
     <t>age_ret</t>
   </si>
   <si>
-    <t>bfactor_classic</t>
-  </si>
-  <si>
-    <t>bfactor_pepra</t>
-  </si>
-  <si>
     <t>2%@55</t>
   </si>
   <si>
@@ -539,6 +533,12 @@
   </si>
   <si>
     <t>C6:G27</t>
+  </si>
+  <si>
+    <t>bfactor_reduced_classic</t>
+  </si>
+  <si>
+    <t>bfactor_reduced_pepra</t>
   </si>
 </sst>
 </file>
@@ -970,6 +970,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
     </xf>
@@ -979,7 +980,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2184,14 +2184,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9147E840-414A-4EF7-8AF7-D7B00A1C58BE}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
@@ -2207,7 +2207,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2227,17 +2227,17 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="D5" s="76" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="76" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>69</v>
+      <c r="D5" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="73" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2245,16 +2245,16 @@
         <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2748,14 +2748,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0846F66D-AF41-4840-B50F-FCBDD98B101F}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
@@ -2770,7 +2770,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2790,17 +2790,17 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="D5" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>68</v>
+      <c r="D5" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="73" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2808,16 +2808,16 @@
         <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3747,22 +3747,22 @@
       <c r="C3" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="73"/>
+      <c r="E3" s="74"/>
     </row>
     <row r="4" spans="3:5">
       <c r="C4" s="61"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
     </row>
     <row r="5" spans="3:5">
       <c r="C5" s="61"/>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="74"/>
+      <c r="E5" s="75"/>
     </row>
     <row r="6" spans="3:5" ht="22.5" customHeight="1">
       <c r="C6" s="61"/>
@@ -4112,28 +4112,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="73"/>
+      <c r="D2" s="74"/>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="75"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="75"/>
-      <c r="C4" s="74" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="74"/>
+      <c r="D4" s="75"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="75"/>
+      <c r="B5" s="76"/>
       <c r="C5" s="51" t="s">
         <v>56</v>
       </c>

</xml_diff>